<commit_message>
Adición estado de cumplimiento
</commit_message>
<xml_diff>
--- a/Matriz de riesgo de activos tecnológicos.xlsx
+++ b/Matriz de riesgo de activos tecnológicos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredobolio/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/clases/sistemasMulti/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50C591E-D293-804E-9DA6-2C55D612139C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACBED22-CE67-9147-AB30-DF3AA33F7FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="500" windowWidth="25460" windowHeight="17660" activeTab="9" xr2:uid="{B2003A59-81C9-0944-8A91-311BFCB0B9B0}"/>
+    <workbookView xWindow="1800" yWindow="500" windowWidth="25460" windowHeight="17660" activeTab="2" xr2:uid="{B2003A59-81C9-0944-8A91-311BFCB0B9B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Fisico" sheetId="1" r:id="rId1"/>
@@ -328,13 +328,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDE1BC"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -477,13 +477,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -524,6 +521,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -845,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FEB84F-75BB-5C49-B35D-879A043FF00D}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection sqref="A1:O18"/>
+      <selection activeCell="B4" sqref="B4:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -868,114 +869,117 @@
     <col min="15" max="15" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:19" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-    </row>
-    <row r="2" spans="1:17" ht="154" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+    </row>
+    <row r="2" spans="1:19" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="6"/>
-    </row>
-    <row r="3" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1</v>
-      </c>
-      <c r="I3" s="9">
-        <v>2</v>
-      </c>
-      <c r="J3" s="9">
-        <v>2</v>
-      </c>
-      <c r="K3" s="9">
-        <v>1</v>
-      </c>
-      <c r="L3" s="9">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9">
-        <v>1</v>
-      </c>
-      <c r="N3" s="9">
-        <v>1</v>
-      </c>
-      <c r="O3" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+    </row>
+    <row r="3" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8">
+        <v>2</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>1</v>
+      </c>
+      <c r="N3" s="8">
+        <v>1</v>
+      </c>
+      <c r="O3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -990,9 +994,9 @@
         <f t="shared" ref="E4:F4" si="0">$C$4*E3</f>
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ref="G4:O4" si="1">$C$4*G3</f>
@@ -1002,9 +1006,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="1"/>
@@ -1031,8 +1035,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+    <row r="5" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1047,9 +1051,9 @@
         <f t="shared" ref="E5:F5" si="2">$C$5*E3</f>
         <v>3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="23">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ref="G5:O5" si="3">$C$5*G3</f>
@@ -1059,11 +1063,11 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="J5" s="4">
+        <v>3</v>
+      </c>
+      <c r="J5" s="23">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -1088,8 +1092,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1104,9 +1108,9 @@
         <f t="shared" ref="E6:F6" si="4">$C$6*E3</f>
         <v>3</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="23">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ref="G6:O6" si="5">$C$6*G3</f>
@@ -1116,11 +1120,11 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="J6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="23">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
@@ -1145,8 +1149,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1161,9 +1165,9 @@
         <f t="shared" ref="E7:F7" si="6">$C$7*E3</f>
         <v>3</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="23">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" ref="G7:O7" si="7">$C$7*G3</f>
@@ -1173,11 +1177,11 @@
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="J7" s="4">
+        <v>3</v>
+      </c>
+      <c r="J7" s="23">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
@@ -1202,8 +1206,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+    <row r="8" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1218,9 +1222,9 @@
         <f t="shared" ref="E8:F8" si="8">$C$8*E3</f>
         <v>3</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="23">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" ref="G8:O8" si="9">$C$8*G3</f>
@@ -1230,11 +1234,11 @@
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="J8" s="4">
+        <v>3</v>
+      </c>
+      <c r="J8" s="23">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
@@ -1259,8 +1263,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1275,9 +1279,9 @@
         <f t="shared" ref="E9:F9" si="10">$C$9*E3</f>
         <v>3</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="23">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" ref="G9:O9" si="11">$C$9*G3</f>
@@ -1287,11 +1291,11 @@
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <f t="shared" si="11"/>
-        <v>6</v>
-      </c>
-      <c r="J9" s="4">
+        <v>3</v>
+      </c>
+      <c r="J9" s="23">
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
@@ -1316,8 +1320,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+    <row r="10" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1332,9 +1336,9 @@
         <f t="shared" ref="E10:F10" si="12">$C$10*E3</f>
         <v>3</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="23">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" ref="G10:O10" si="13">$C$10*G3</f>
@@ -1344,11 +1348,11 @@
         <f t="shared" si="13"/>
         <v>3</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f t="shared" si="13"/>
-        <v>6</v>
-      </c>
-      <c r="J10" s="4">
+        <v>3</v>
+      </c>
+      <c r="J10" s="23">
         <f t="shared" si="13"/>
         <v>6</v>
       </c>
@@ -1373,8 +1377,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1389,9 +1393,9 @@
         <f t="shared" ref="E11:F11" si="14">$C$11*E3</f>
         <v>3</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="23">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ref="G11:O11" si="15">$C$11*G3</f>
@@ -1401,11 +1405,11 @@
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <f t="shared" si="15"/>
-        <v>6</v>
-      </c>
-      <c r="J11" s="4">
+        <v>3</v>
+      </c>
+      <c r="J11" s="23">
         <f t="shared" si="15"/>
         <v>6</v>
       </c>
@@ -1430,8 +1434,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1446,9 +1450,9 @@
         <f t="shared" ref="E12:F12" si="16">$C$12*E3</f>
         <v>3</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="23">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" ref="G12:O12" si="17">$C$12*G3</f>
@@ -1458,11 +1462,11 @@
         <f t="shared" si="17"/>
         <v>3</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f t="shared" si="17"/>
-        <v>6</v>
-      </c>
-      <c r="J12" s="4">
+        <v>3</v>
+      </c>
+      <c r="J12" s="23">
         <f t="shared" si="17"/>
         <v>6</v>
       </c>
@@ -1487,8 +1491,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1503,9 +1507,9 @@
         <f t="shared" ref="E13:F13" si="18">$C$13*E3</f>
         <v>3</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="23">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" ref="G13:O13" si="19">$C$13*G3</f>
@@ -1515,11 +1519,11 @@
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <f t="shared" si="19"/>
-        <v>6</v>
-      </c>
-      <c r="J13" s="4">
+        <v>3</v>
+      </c>
+      <c r="J13" s="23">
         <f t="shared" si="19"/>
         <v>6</v>
       </c>
@@ -1544,8 +1548,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+    <row r="14" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1560,9 +1564,9 @@
         <f t="shared" ref="E14:F14" si="20">$C$14*E3</f>
         <v>3</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="23">
         <f t="shared" si="20"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" ref="G14:O14" si="21">$C$14*G3</f>
@@ -1572,11 +1576,11 @@
         <f t="shared" si="21"/>
         <v>3</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <f t="shared" si="21"/>
-        <v>6</v>
-      </c>
-      <c r="J14" s="4">
+        <v>3</v>
+      </c>
+      <c r="J14" s="23">
         <f t="shared" si="21"/>
         <v>6</v>
       </c>
@@ -1601,8 +1605,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+    <row r="15" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1617,9 +1621,9 @@
         <f t="shared" ref="E15:F15" si="22">$C$15*E3</f>
         <v>3</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="23">
         <f t="shared" si="22"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" ref="G15:O15" si="23">$C$15*G3</f>
@@ -1629,11 +1633,11 @@
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <f t="shared" si="23"/>
-        <v>6</v>
-      </c>
-      <c r="J15" s="4">
+        <v>3</v>
+      </c>
+      <c r="J15" s="23">
         <f t="shared" si="23"/>
         <v>6</v>
       </c>
@@ -1658,8 +1662,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+    <row r="16" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1674,9 +1678,9 @@
         <f t="shared" ref="E16:F16" si="24">$C$16*E3</f>
         <v>3</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="23">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" ref="G16:N16" si="25">$C$16*G3</f>
@@ -1686,11 +1690,11 @@
         <f t="shared" si="25"/>
         <v>3</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <f t="shared" si="25"/>
-        <v>6</v>
-      </c>
-      <c r="J16" s="4">
+        <v>3</v>
+      </c>
+      <c r="J16" s="23">
         <f t="shared" si="25"/>
         <v>6</v>
       </c>
@@ -1716,7 +1720,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1731,9 +1735,9 @@
         <f t="shared" ref="E17:F17" si="26">$C$17*E3</f>
         <v>3</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="23">
         <f t="shared" si="26"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" ref="G17:O17" si="27">$C$17*G3</f>
@@ -1743,11 +1747,11 @@
         <f t="shared" si="27"/>
         <v>3</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <f t="shared" si="27"/>
-        <v>6</v>
-      </c>
-      <c r="J17" s="4">
+        <v>3</v>
+      </c>
+      <c r="J17" s="23">
         <f t="shared" si="27"/>
         <v>6</v>
       </c>
@@ -1773,7 +1777,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1788,9 +1792,9 @@
         <f t="shared" ref="E18:F18" si="28">$C$18*E3</f>
         <v>3</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="23">
         <f t="shared" si="28"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" ref="G18:O18" si="29">$C$18*G3</f>
@@ -1800,11 +1804,11 @@
         <f t="shared" si="29"/>
         <v>3</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <f t="shared" si="29"/>
-        <v>6</v>
-      </c>
-      <c r="J18" s="4">
+        <v>3</v>
+      </c>
+      <c r="J18" s="23">
         <f t="shared" si="29"/>
         <v>6</v>
       </c>
@@ -1843,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC006D5-FE2F-4248-8D81-9EDA418C9A72}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A2" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1860,71 +1864,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9">
-        <v>2</v>
-      </c>
-      <c r="H3" s="9">
-        <v>3</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="A3" s="18"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1957,7 +1961,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>59</v>
       </c>
@@ -1990,7 +1994,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>60</v>
       </c>
@@ -2023,7 +2027,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
@@ -2056,7 +2060,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>62</v>
       </c>
@@ -2103,7 +2107,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2119,121 +2123,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="194" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>3</v>
-      </c>
-      <c r="F3" s="9">
-        <v>3</v>
-      </c>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>3</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3">
         <f>$C$4*D3</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="23">
         <f t="shared" ref="E4:H4" si="0">$C$4*E3</f>
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
+        <v>6</v>
+      </c>
+      <c r="F4" s="23">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3">
         <f>$C$5*D3</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="23">
         <f t="shared" ref="E5:H5" si="1">$C$5*E3</f>
-        <v>3</v>
-      </c>
-      <c r="F5" s="3">
+        <v>6</v>
+      </c>
+      <c r="F5" s="23">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2262,7 +2266,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2291,7 +2295,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2320,7 +2324,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2349,7 +2353,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2360,11 +2364,11 @@
         <f>$C$10*D3</f>
         <v>2</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="23">
         <f t="shared" ref="E10:H10" si="6">$C$10*E3</f>
         <v>6</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="23">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -2378,7 +2382,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2401,13 +2405,13 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="23">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2436,7 +2440,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -2465,7 +2469,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2494,7 +2498,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -2523,7 +2527,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2552,7 +2556,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2581,7 +2585,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2623,8 +2627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7B8568-FD94-6B45-BA8B-820A92EC9717}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2634,61 +2638,61 @@
     <col min="3" max="3" width="3.83203125" customWidth="1"/>
     <col min="4" max="4" width="5.33203125" customWidth="1"/>
     <col min="5" max="5" width="4.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="195" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>3</v>
-      </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2713,7 +2717,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -2738,7 +2742,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2763,7 +2767,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2788,7 +2792,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2813,7 +2817,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2838,7 +2842,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2863,7 +2867,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2888,7 +2892,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2913,7 +2917,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -2938,7 +2942,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2963,7 +2967,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -2988,7 +2992,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3013,7 +3017,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3038,7 +3042,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -3077,7 +3081,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3091,49 +3095,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>3</v>
-      </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3154,7 +3158,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3175,7 +3179,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -3196,7 +3200,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -3217,7 +3221,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3238,7 +3242,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -3259,7 +3263,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3280,7 +3284,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -3301,7 +3305,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -3322,7 +3326,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -3343,7 +3347,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -3364,7 +3368,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -3385,7 +3389,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3406,7 +3410,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3427,7 +3431,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -3461,8 +3465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2A3B71-8E89-9446-9E44-F5E8FF082C7F}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A2" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3475,56 +3479,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="163" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9">
-        <v>3</v>
+      <c r="A3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3533,7 +3537,7 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ref="D4:G4" si="0">$C$4*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
@@ -3541,15 +3545,15 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3558,7 +3562,7 @@
       </c>
       <c r="D5" s="3">
         <f>$C$5*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ref="E5:F5" si="1">$C$5*E3</f>
@@ -3566,15 +3570,15 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ref="G5" si="2">$C$5*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -3583,7 +3587,7 @@
       </c>
       <c r="D6" s="3">
         <f>$C$6*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ref="E6:F6" si="3">$C$6*E3</f>
@@ -3591,15 +3595,15 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ref="G6" si="4">$C$6*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -3608,7 +3612,7 @@
       </c>
       <c r="D7" s="3">
         <f>$C$7*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ref="E7:F7" si="5">$C$7*E3</f>
@@ -3616,15 +3620,15 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" ref="G7" si="6">$C$7*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3633,7 +3637,7 @@
       </c>
       <c r="D8" s="3">
         <f>$C$8*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ref="E8:F8" si="7">$C$8*E3</f>
@@ -3641,15 +3645,15 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" ref="G8" si="8">$C$8*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -3658,7 +3662,7 @@
       </c>
       <c r="D9" s="3">
         <f>$C$9*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ref="E9:F9" si="9">$C$9*E3</f>
@@ -3666,90 +3670,90 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" ref="G9" si="10">$C$9*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <f>$C$10*D3</f>
-        <v>6</v>
-      </c>
-      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5">
         <f t="shared" ref="E10:F10" si="11">$C$10*E3</f>
         <v>6</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" ref="G10" si="12">$C$10*G3</f>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5">
         <f>$C$11*D3</f>
-        <v>2</v>
-      </c>
-      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
         <f t="shared" ref="E11:F11" si="13">$C$11*E3</f>
-        <v>2</v>
-      </c>
-      <c r="F11" s="3">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5">
         <f t="shared" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" ref="G11" si="14">$C$11*G3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5">
         <f>$C$12*D3</f>
-        <v>4</v>
-      </c>
-      <c r="E12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5">
         <f t="shared" ref="E12:F12" si="15">$C$12*E3</f>
-        <v>4</v>
-      </c>
-      <c r="F12" s="3">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="G12" s="4">
+        <v>3</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" ref="G12" si="16">$C$12*G3</f>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -3758,7 +3762,7 @@
       </c>
       <c r="D13" s="3">
         <f>$C$13*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ref="E13:F13" si="17">$C$13*E3</f>
@@ -3766,15 +3770,15 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" ref="G13" si="18">$C$13*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -3783,7 +3787,7 @@
       </c>
       <c r="D14" s="3">
         <f>$C$14*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ref="E14:F14" si="19">$C$14*E3</f>
@@ -3791,15 +3795,15 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" ref="G14" si="20">$C$14*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -3808,7 +3812,7 @@
       </c>
       <c r="D15" s="3">
         <f>$C$15*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ref="E15:F15" si="21">$C$15*E3</f>
@@ -3816,15 +3820,15 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="21"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" ref="G15" si="22">$C$15*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3833,7 +3837,7 @@
       </c>
       <c r="D16" s="3">
         <f>$C$16*D3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ref="E16:F16" si="23">$C$16*E3</f>
@@ -3841,61 +3845,61 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" ref="G16" si="24">$C$16*G3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5">
         <f>$C$17*D3</f>
-        <v>2</v>
-      </c>
-      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
         <f t="shared" ref="E17:F17" si="25">$C$17*E3</f>
-        <v>2</v>
-      </c>
-      <c r="F17" s="3">
+        <v>6</v>
+      </c>
+      <c r="F17" s="5">
         <f t="shared" si="25"/>
-        <v>2</v>
-      </c>
-      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5">
         <f t="shared" ref="G17" si="26">$C$17*G3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="2">
         <v>3</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="5">
         <f>$C$18*D3</f>
-        <v>6</v>
-      </c>
-      <c r="E18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
         <f t="shared" ref="E18:F18" si="27">$C$18*E3</f>
         <v>6</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="5">
         <f t="shared" si="27"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" ref="G18" si="28">$C$18*G3</f>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3912,8 +3916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8659AAD9-68F8-DE44-8C06-82145D587576}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A2" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3929,63 +3933,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>3</v>
-      </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9">
-        <v>2</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1</v>
+      <c r="A3" s="18"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -4010,11 +4014,11 @@
       </c>
       <c r="H4" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -4039,11 +4043,11 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -4068,11 +4072,11 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -4097,11 +4101,11 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -4126,11 +4130,11 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -4155,11 +4159,11 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4184,11 +4188,11 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -4213,11 +4217,11 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -4242,11 +4246,11 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -4271,11 +4275,11 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -4300,11 +4304,11 @@
       </c>
       <c r="H14" s="3">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -4329,11 +4333,11 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4358,11 +4362,11 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4387,11 +4391,11 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -4416,7 +4420,7 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -4434,7 +4438,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4451,70 +4455,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="188" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9">
-        <v>3</v>
-      </c>
-      <c r="H3" s="9">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="A3" s="18"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>3</v>
+      </c>
+      <c r="H3" s="8">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -4547,7 +4551,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -4580,7 +4584,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -4613,7 +4617,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -4646,7 +4650,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -4679,7 +4683,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -4712,7 +4716,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4745,7 +4749,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -4778,7 +4782,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -4811,7 +4815,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -4844,7 +4848,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -4877,7 +4881,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -4910,7 +4914,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4943,7 +4947,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4976,7 +4980,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -5022,8 +5026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D33FFE-616E-D844-B824-45F5615670A4}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+    <sheetView topLeftCell="A2" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5038,56 +5042,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="A3" s="18"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -5112,7 +5116,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -5137,7 +5141,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -5162,7 +5166,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -5187,7 +5191,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -5212,7 +5216,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -5237,7 +5241,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -5262,7 +5266,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -5287,7 +5291,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -5312,7 +5316,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -5337,7 +5341,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -5362,7 +5366,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -5387,7 +5391,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -5412,7 +5416,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -5437,7 +5441,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -5476,7 +5480,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection sqref="A1:N8"/>
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5496,106 +5500,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:16" ht="154" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="10"/>
+      <c r="P2" s="9"/>
     </row>
     <row r="3" spans="1:16" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9">
-        <v>2</v>
-      </c>
-      <c r="J3" s="9">
-        <v>2</v>
-      </c>
-      <c r="K3" s="9">
-        <v>1</v>
-      </c>
-      <c r="L3" s="9">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9">
-        <v>1</v>
-      </c>
-      <c r="N3" s="9">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2</v>
+      </c>
+      <c r="J3" s="8">
+        <v>2</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>1</v>
+      </c>
+      <c r="N3" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
@@ -5648,7 +5652,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>59</v>
       </c>
@@ -5701,7 +5705,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>60</v>
       </c>
@@ -5754,7 +5758,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
@@ -5807,7 +5811,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>